<commit_message>
quase la, falta implementar jacobi
</commit_message>
<xml_diff>
--- a/entrada.xlsx
+++ b/entrada.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://insper-my.sharepoint.com/personal/caiofrs_insper_edu_br/Documents/Insper/2_TERMOSOLIDOS/APS/2021/APS 3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Disciplinas\5-semestre\transferência de calor e mecânica dos sólidos\APS3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_B83576887843B5F308FB41B3B0A882DC2AEE8E3C" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C48F6A4B-2E11-40DF-BD96-CB6BDBFD4F71}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9567E229-A051-4742-8BB2-C4BB0953D4C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nos" sheetId="1" r:id="rId1"/>
@@ -507,18 +507,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="11.6640625" customWidth="1"/>
+    <col min="1" max="4" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
@@ -530,7 +530,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -540,32 +540,76 @@
       <c r="C2" s="2"/>
       <c r="D2" s="9">
         <f>COUNT(A2:A1048576)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
         <v>0</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0.4</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <v>3</v>
+      </c>
+      <c r="B5" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>4</v>
+      </c>
+      <c r="B6" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>3</v>
+      </c>
+      <c r="B7" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>2</v>
+      </c>
+      <c r="B8" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>1</v>
+      </c>
+      <c r="B9" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>2</v>
+      </c>
+      <c r="B10" s="10">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -574,18 +618,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B4"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="11.6640625" customWidth="1"/>
+    <col min="1" max="7" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -603,7 +647,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -614,15 +658,16 @@
         <v>210000000000</v>
       </c>
       <c r="D2" s="3">
-        <v>2.0000000000000001E-4</v>
+        <f>0.15*0.15</f>
+        <v>2.2499999999999999E-2</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="7">
         <f>COUNT(A2:A1048576)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -633,24 +678,221 @@
         <v>210000000000</v>
       </c>
       <c r="D3" s="3">
-        <v>2.0000000000000001E-4</v>
+        <f t="shared" ref="D3:D17" si="0">0.15*0.15</f>
+        <v>2.2499999999999999E-2</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3">
+        <v>210000000000</v>
+      </c>
+      <c r="D4" s="3">
+        <f t="shared" si="0"/>
+        <v>2.2499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3">
+        <v>210000000000</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" si="0"/>
+        <v>2.2499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>6</v>
+      </c>
+      <c r="C6" s="3">
+        <v>210000000000</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" si="0"/>
+        <v>2.2499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>7</v>
+      </c>
+      <c r="C7" s="3">
+        <v>210000000000</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="0"/>
+        <v>2.2499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3">
+        <v>210000000000</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="0"/>
+        <v>2.2499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
         <v>1</v>
       </c>
-      <c r="C4" s="3">
-        <v>210000000000</v>
-      </c>
-      <c r="D4" s="3">
-        <v>2.0000000000000001E-4</v>
+      <c r="C9" s="3">
+        <v>210000000000</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="0"/>
+        <v>2.2499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>2</v>
+      </c>
+      <c r="B10" s="2">
+        <v>8</v>
+      </c>
+      <c r="C10" s="3">
+        <v>210000000000</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="0"/>
+        <v>2.2499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>2</v>
+      </c>
+      <c r="B11" s="2">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3">
+        <v>210000000000</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="0"/>
+        <v>2.2499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>3</v>
+      </c>
+      <c r="B12" s="2">
+        <v>9</v>
+      </c>
+      <c r="C12" s="3">
+        <v>210000000000</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="0"/>
+        <v>2.2499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>9</v>
+      </c>
+      <c r="B13" s="2">
+        <v>4</v>
+      </c>
+      <c r="C13" s="3">
+        <v>210000000000</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="0"/>
+        <v>2.2499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>4</v>
+      </c>
+      <c r="B14" s="2">
+        <v>6</v>
+      </c>
+      <c r="C14" s="3">
+        <v>210000000000</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="0"/>
+        <v>2.2499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>9</v>
+      </c>
+      <c r="B15" s="2">
+        <v>6</v>
+      </c>
+      <c r="C15" s="3">
+        <v>210000000000</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="0"/>
+        <v>2.2499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>8</v>
+      </c>
+      <c r="B16" s="2">
+        <v>9</v>
+      </c>
+      <c r="C16" s="3">
+        <v>210000000000</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="0"/>
+        <v>2.2499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>9</v>
+      </c>
+      <c r="B17" s="2">
+        <v>7</v>
+      </c>
+      <c r="C17" s="3">
+        <v>210000000000</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" si="0"/>
+        <v>2.2499999999999999E-2</v>
       </c>
     </row>
   </sheetData>
@@ -664,15 +906,15 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A4" sqref="A4:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="11.6640625" customWidth="1"/>
+    <col min="1" max="5" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>8</v>
       </c>
@@ -687,169 +929,175 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
       </c>
       <c r="C2" s="2">
-        <v>150</v>
+        <v>2000</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="9">
         <f>COUNT(A2:A1048576)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
       </c>
       <c r="C3" s="2">
-        <v>-100</v>
+        <v>-10000</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2000</v>
+      </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -866,15 +1114,15 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="11.6640625" customWidth="1"/>
+    <col min="1" max="4" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="28.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>8</v>
       </c>
@@ -886,7 +1134,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -896,20 +1144,20 @@
       <c r="C2" s="2"/>
       <c r="D2" s="9">
         <f>COUNT(A2:A1048576)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -919,113 +1167,131 @@
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <v>3</v>
+      </c>
+      <c r="B5" s="10">
+        <v>2</v>
+      </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2</v>
+      </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2</v>
+      </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>

</xml_diff>